<commit_message>
mapeo inscripcion de clave dinamica
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/clavedinamica/InscribirClaveDinamica.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/clavedinamica/InscribirClaveDinamica.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUTOMATIZACION JAVA\PROYECTOS GRADLE\PROYECTOS NUEVA APP\AW1059001_APPSucursalVirtualPersonas_Test\APP_PERSONAS\src\test\resources\datadriven\autenticacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695"/>
+    <workbookView windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -58,13 +53,25 @@
     <t>validarClave</t>
   </si>
   <si>
+    <t>nombrePersonalizado</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>tipoCorreo</t>
+  </si>
+  <si>
+    <t>numeroCelular</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>1037655531</t>
-  </si>
-  <si>
-    <t>userqa10</t>
+    <t>67652517</t>
+  </si>
+  <si>
+    <t>AutoTest1</t>
   </si>
   <si>
     <t>1234</t>
@@ -91,6 +98,18 @@
     <t>ACTIVO</t>
   </si>
   <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>scampo@todo1.net</t>
+  </si>
+  <si>
+    <t>Laboral</t>
+  </si>
+  <si>
+    <t>3145678956</t>
+  </si>
+  <si>
     <t>Orientacion</t>
   </si>
   <si>
@@ -137,43 +156,19 @@
   </si>
   <si>
     <t>Consultas</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1111</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>95400152</t>
-  </si>
-  <si>
-    <t>sandrita69</t>
-  </si>
-  <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>0370</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>58156994</t>
-  </si>
-  <si>
-    <t>invictus01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -189,21 +184,158 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,12 +354,211 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -246,34 +577,345 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Título 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
+    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
+    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Moneda" xfId="5" builtinId="4"/>
+    <cellStyle name="Coma" xfId="6" builtinId="3"/>
+    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
+    <cellStyle name="Hipervínculo" xfId="8" builtinId="8"/>
+    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21"/>
+    <cellStyle name="Nota" xfId="11" builtinId="10"/>
+    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
+    <cellStyle name="Texto de advertencia" xfId="13" builtinId="11"/>
+    <cellStyle name="Título" xfId="14" builtinId="15"/>
+    <cellStyle name="Texto explicativo" xfId="15" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="16" builtinId="16"/>
+    <cellStyle name="Título 4" xfId="17" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="18" builtinId="20"/>
+    <cellStyle name="Cálculo" xfId="19" builtinId="22"/>
+    <cellStyle name="Celda de comprobación" xfId="20" builtinId="23"/>
+    <cellStyle name="Celda vinculada" xfId="21" builtinId="24"/>
+    <cellStyle name="Total" xfId="22" builtinId="25"/>
+    <cellStyle name="Correcto" xfId="23" builtinId="26"/>
+    <cellStyle name="40% - Énfasis5" xfId="24" builtinId="47"/>
+    <cellStyle name="Incorrecto" xfId="25" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="26" builtinId="28"/>
+    <cellStyle name="20% - Énfasis5" xfId="27" builtinId="46"/>
+    <cellStyle name="Énfasis1" xfId="28" builtinId="29"/>
+    <cellStyle name="20% - Énfasis1" xfId="29" builtinId="30"/>
+    <cellStyle name="60% - Énfasis1" xfId="30" builtinId="32"/>
+    <cellStyle name="20% - Énfasis6" xfId="31" builtinId="50"/>
+    <cellStyle name="Énfasis2" xfId="32" builtinId="33"/>
+    <cellStyle name="20% - Énfasis2" xfId="33" builtinId="34"/>
+    <cellStyle name="40% - Énfasis2" xfId="34" builtinId="35"/>
+    <cellStyle name="60% - Énfasis2" xfId="35" builtinId="36"/>
+    <cellStyle name="Énfasis3" xfId="36" builtinId="37"/>
+    <cellStyle name="20% - Énfasis3" xfId="37" builtinId="38"/>
+    <cellStyle name="40% - Énfasis3" xfId="38" builtinId="39"/>
+    <cellStyle name="60% - Énfasis3" xfId="39" builtinId="40"/>
+    <cellStyle name="Énfasis4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Énfasis4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Énfasis4" xfId="42" builtinId="43"/>
+    <cellStyle name="60% - Énfasis4" xfId="43" builtinId="44"/>
+    <cellStyle name="Énfasis5" xfId="44" builtinId="45"/>
+    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48"/>
+    <cellStyle name="Énfasis6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
+    <cellStyle name="Normal 2" xfId="48"/>
+    <cellStyle name="60% - Énfasis6" xfId="49" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -531,247 +1173,191 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="6" customWidth="1"/>
-    <col min="2" max="6" width="14.375" style="6" customWidth="1"/>
-    <col min="7" max="8" width="11" style="6"/>
-    <col min="9" max="9" width="18.375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="22.125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="14.375" style="6" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="11" style="6"/>
+    <col min="1" max="1" width="11.125" style="2" customWidth="1"/>
+    <col min="2" max="6" width="14.375" style="2" customWidth="1"/>
+    <col min="7" max="8" width="11" style="2"/>
+    <col min="9" max="9" width="18.375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="22.125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.625" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="5" t="s">
+    <row r="2" spans="1:16">
+      <c r="A2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="C2" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="E2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="F2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>22</v>
       </c>
+      <c r="I2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>22</v>
-      </c>
+    <row r="3" spans="1:16">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>22</v>
-      </c>
+    <row r="4" spans="2:15">
+      <c r="B4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>22</v>
-      </c>
+    <row r="5" s="1" customFormat="1" spans="3:12">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J5">
+      <formula1>Listas!$A$2:$A$3</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Listas!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:J5</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="10.625" customWidth="1"/>
     <col min="2" max="2" width="14.875" customWidth="1"/>
@@ -781,70 +1367,71 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambio en el encarpetado
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/clavedinamica/InscribirClaveDinamica.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/clavedinamica/InscribirClaveDinamica.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20130" windowHeight="7425"/>
+    <workbookView windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -68,16 +68,16 @@
     <t>1</t>
   </si>
   <si>
-    <t>67652517</t>
-  </si>
-  <si>
-    <t>testing10</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>4321</t>
+    <t>22468280</t>
+  </si>
+  <si>
+    <t>pruebauser01</t>
+  </si>
+  <si>
+    <t>6789</t>
+  </si>
+  <si>
+    <t>9876</t>
   </si>
   <si>
     <t>Acierto</t>
@@ -98,10 +98,10 @@
     <t>ACTIVO</t>
   </si>
   <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>scampo@todo1.net</t>
+    <t>User01</t>
+  </si>
+  <si>
+    <t>jfernandez@todo1.net</t>
   </si>
   <si>
     <t>Laboral</t>
@@ -164,9 +164,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -191,6 +191,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -199,7 +228,61 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,47 +296,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,51 +314,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -356,181 +356,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,6 +591,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -610,22 +628,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -645,20 +648,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -691,153 +691,153 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="34" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -852,6 +852,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -862,55 +863,55 @@
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Título 3" xfId="1" builtinId="18"/>
-    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
-    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
-    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Moneda" xfId="5" builtinId="4"/>
-    <cellStyle name="Coma" xfId="6" builtinId="3"/>
-    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
-    <cellStyle name="Hipervínculo" xfId="8" builtinId="8"/>
-    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21"/>
-    <cellStyle name="Nota" xfId="11" builtinId="10"/>
-    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
-    <cellStyle name="Texto de advertencia" xfId="13" builtinId="11"/>
-    <cellStyle name="Título" xfId="14" builtinId="15"/>
-    <cellStyle name="Texto explicativo" xfId="15" builtinId="53"/>
-    <cellStyle name="Título 1" xfId="16" builtinId="16"/>
-    <cellStyle name="Título 4" xfId="17" builtinId="19"/>
-    <cellStyle name="Entrada" xfId="18" builtinId="20"/>
-    <cellStyle name="Cálculo" xfId="19" builtinId="22"/>
-    <cellStyle name="Celda de comprobación" xfId="20" builtinId="23"/>
-    <cellStyle name="Celda vinculada" xfId="21" builtinId="24"/>
-    <cellStyle name="Total" xfId="22" builtinId="25"/>
-    <cellStyle name="Correcto" xfId="23" builtinId="26"/>
-    <cellStyle name="40% - Énfasis5" xfId="24" builtinId="47"/>
-    <cellStyle name="Incorrecto" xfId="25" builtinId="27"/>
-    <cellStyle name="Neutro" xfId="26" builtinId="28"/>
-    <cellStyle name="20% - Énfasis5" xfId="27" builtinId="46"/>
-    <cellStyle name="Énfasis1" xfId="28" builtinId="29"/>
-    <cellStyle name="20% - Énfasis1" xfId="29" builtinId="30"/>
-    <cellStyle name="60% - Énfasis1" xfId="30" builtinId="32"/>
-    <cellStyle name="20% - Énfasis6" xfId="31" builtinId="50"/>
-    <cellStyle name="Énfasis2" xfId="32" builtinId="33"/>
-    <cellStyle name="20% - Énfasis2" xfId="33" builtinId="34"/>
-    <cellStyle name="40% - Énfasis2" xfId="34" builtinId="35"/>
-    <cellStyle name="60% - Énfasis2" xfId="35" builtinId="36"/>
-    <cellStyle name="Énfasis3" xfId="36" builtinId="37"/>
-    <cellStyle name="20% - Énfasis3" xfId="37" builtinId="38"/>
-    <cellStyle name="40% - Énfasis3" xfId="38" builtinId="39"/>
-    <cellStyle name="60% - Énfasis3" xfId="39" builtinId="40"/>
-    <cellStyle name="Énfasis4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Énfasis4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Énfasis4" xfId="42" builtinId="43"/>
-    <cellStyle name="60% - Énfasis4" xfId="43" builtinId="44"/>
-    <cellStyle name="Énfasis5" xfId="44" builtinId="45"/>
-    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48"/>
-    <cellStyle name="Énfasis6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
-    <cellStyle name="Normal 2" xfId="48"/>
-    <cellStyle name="60% - Énfasis6" xfId="49" builtinId="52"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="Normal 2" xfId="32"/>
+    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="40" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="41" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="43" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="44" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="45" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="46" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="47" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="48" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="49" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1181,8 +1182,8 @@
   <sheetPr/>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="4"/>
@@ -1248,22 +1249,22 @@
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="6" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="6" t="s">
@@ -1278,22 +1279,22 @@
       <c r="J2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="21" t="s">
         <v>26</v>
       </c>
       <c r="M2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="P2" s="16" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1331,7 +1332,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
-      <c r="I5" s="16"/>
+      <c r="I5" s="17"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -1342,6 +1343,9 @@
       <formula1>Listas!$A$2:$A$3</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" display="jfernandez@todo1.net"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>

</xml_diff>